<commit_message>
Gompertz functions used to find unbiased abundance estimates
</commit_message>
<xml_diff>
--- a/AllPattern.xlsx
+++ b/AllPattern.xlsx
@@ -10,18 +10,21 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sites" sheetId="2" r:id="rId2"/>
     <sheet name="CommunityTypes" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Table" sheetId="4" r:id="rId4"/>
+    <sheet name="Datasets" sheetId="5" r:id="rId5"/>
+    <sheet name="Sources" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CommunityTypes!$A$1:$A$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sites!$A$1:$A$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sources!$A$1:$A$91</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="274">
   <si>
     <t>Hubbard</t>
   </si>
@@ -599,12 +602,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>Time Series</t>
-  </si>
-  <si>
-    <t>% differenceinPattern</t>
-  </si>
-  <si>
     <t>Konza LTER</t>
   </si>
   <si>
@@ -681,14 +678,353 @@
   </si>
   <si>
     <t>JornadaCW</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Holmes, R.T, Sillett, S., Sherry, T.W., and Sturges, F.W. 2010. Bird Abundances at Hubbard Brook (1969-2010) and on three replicate plots (1986-2000) in the White Mountain National Forest. Corvallis, OR: Forest Science Data Bank: 81. [Database]. http://www.hubbardbrook.org/data/dataset.php?id=81</t>
+  </si>
+  <si>
+    <t>Vickery, William L., and Thomas D. Nudds. 1984. Detection of Density-Dependent Effects in Annual Duck Censuses. Ecology 65:96–104. http://dx.doi.org/10.2307/1939462</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sandercock, B.K. (2009). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bird Populations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Konza Prarie LTER: CBP01. [Database].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dickson, J.G., Conner, R.N. &amp; Williamson, J.H. (1993). Neotropical Migratory Bird Communities in a Developing Pine Plantation. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1993 Procedings on the Annual Conference. SEAFWA.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gaston, K.J. &amp; Blackburn, T.M. (Eds.). (2007). Appendix II: Eastern Wood Breeding Bird Data. In: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pattern and Process in Macroecology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Blackwell Science Ltd, pp. 355–357.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sauer, J.R., Hines, J.E., Gough, G., Thomas, I. &amp; Peterjohn, B.G. (1997). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The North American Breeding Bird Survey Results and Analysis. Version 96.4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Patuxent Wildlife Research Center, Laurel, MD.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mountain Bird Watch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. (2010). . Vermont Center for Ecostudies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Robert B. Waide. (2012). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avian populations Long-Term Monitoring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Luquillo LTER project of the Institute for Tropical Ecosystem Studies: Bird abundance - point counts [Database].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Henderson, P. (2010). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The marine community at Hinkley Point</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. The Global Population Dynamics Database Version 2. NERC Centre for Population Biology, Imperial College.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Heessen, H.J.L. (1996). Time-series data for a selection of forty fish species caught during the International Bottom Trawl Survey. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ICES J. Mar. Sci.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 53, 1079–1084.</t>
+    </r>
+  </si>
+  <si>
+    <t>Henry S. Fitch. (2006). Historic and Legacy Data on Snakes. Kansas Biological Survey., University of Kansas Field Station.</t>
+  </si>
+  <si>
+    <t>R. Haven Wiley. (2005). Population estimates of Appalachian salamanders. Coweeta LTER: knb-lter-cwt.1044.4 [Database].</t>
+  </si>
+  <si>
+    <t>Reagan, D. (2010). Anole Population Dynamics. Luquillo LTER project of the Institute for Tropical Ecosystem Studies: Anole Vertical Transects (tower data) [Database].</t>
+  </si>
+  <si>
+    <t>Edwin S. George Reserve Turtles. (2010). The Global Population Dynamics Database Version 2. NERC Centre for Population Biology, Imperial College.</t>
+  </si>
+  <si>
+    <t>Cody, M.L. &amp; Smallwood, J.A. (1996). Long-Term Studies of Vertebrate Communities. Academic Press.</t>
+  </si>
+  <si>
+    <t>Beddington, J.R., Beverton, R. &amp; Lavigne, D.M. (Eds.). (1985). Marine Mammals and Fisheries. George Allen and Unwin Ltd., London.</t>
+  </si>
+  <si>
+    <t>Holmes, R.T. (1997). Long-term trends in abundance of Lepidoptera larvae in northern hardwood forests. Corvallis, OR: Forest Science Data Bank: 82 [Database], Hubbard Brook Experimental Forest.</t>
+  </si>
+  <si>
+    <t>Anderson, J. (2003). Arthropod Pitfall Traps at LTER II NPP sites. Jornada LTER: ARTHPIT3 [Database].</t>
+  </si>
+  <si>
+    <t>Willig, M. &amp; Bloch, C.P. (2004). Community Ecology of Land Snails Survey (Long-term population dynamics of snails in the tabonuco forest). Luquillo LTER project of the Institute for Tropical Ecosystem Studies: Lterdb107 [Database].</t>
+  </si>
+  <si>
+    <t>Rudstam, L. &amp; Mills, E. (2008). Zooplankton survey of Oneida Lake, New York, 1975 - 2006.</t>
+  </si>
+  <si>
+    <t>Raimondi, P., Blanchette, C. &amp; Miner, M. (2009). MARINe Core Surveys: Species Counts. PISCO: Intertidal: MLPA baseline: Central Coast: MLPA_intertidal.81.2 [Database].</t>
+  </si>
+  <si>
+    <t>Pollard, E., Hall, M.L. &amp; Bibby, T.J. (1986). Monitoring the Abundance of Butterflies 1976-1985. Joint Nature Conservation Committee.</t>
+  </si>
+  <si>
+    <t>Ernest, S.K.M., Valone, T.J. &amp; Brown, J.H. (2009). Long-term monitoring and experimental manipulation of a Chihuahuan Desert ecosystem near Portal, Arizona, USA. Ecology, 90, 1708–1708.</t>
+  </si>
+  <si>
+    <t>Friggens, M. (2008). Small Mammal Mark-Recapture Population Dynamics at Core Research Sites at the Sevilleta National Wildlife Refuge, New Mexico. Albuquerque, NM: Sevilleta Long Term Ecological Research Site Database: SEV008.</t>
+  </si>
+  <si>
+    <t>Kaufman, D.W. (2010). Seasonal summary of numbers of small mammals on the LTER traplines in prairie. Konza Prarie LTER: CSM04.</t>
+  </si>
+  <si>
+    <t>Bartel, R.A., Knowlton, F.F. &amp; Stoddart, L.C. (2005). Mammal abundance indices in the northern portion of the Great Basin, 1962–1993. Ecology, 86, 3130.</t>
+  </si>
+  <si>
+    <t>PortalSummer</t>
+  </si>
+  <si>
+    <t>Bestelmeyer, B. (2007). Small Mammal Exclosure Study. Jornada LTER: smesrdnt.</t>
+  </si>
+  <si>
+    <t>Peters, D. (2008). Spatial and Temporal Patterns of Net Primary Production    in Chihuahuan Desert Ecosystems (NPP Study). Jornada LTER: nppqdbio.</t>
+  </si>
+  <si>
+    <t>Merritt, J. (1999). Long Term Mammal Data from Powdermill Biological Station. Virginia Coast Reserve Long-Term Ecological Research Project Data Publication knb-lter-vcr.67.11.</t>
+  </si>
+  <si>
+    <t>Williamson, M. (1983). The Land-Bird Community of Skokholm: Ordination and Turnover. Oikos, 41, 378–384.</t>
+  </si>
+  <si>
+    <t>Stapp, P. (2006). SGS-LTER Long-Term Monitoring Project: Small Mammals on Trapping Webs [WWW Document]. Shortgrass Steppe LTER: LTMntrSmlMamWebs. URL http://sgs.cnr.colostate.edu/dataset_view.aspx?id=LTMntrSmlMamWebs</t>
+  </si>
+  <si>
+    <t>Fryxell, J.M., Falls, J.B., Falls, E.A. &amp; Brooks, R.J. (1998). Long-Term Dynamics of Small-Mammal Populations in Ontario. Ecology, 79, 213–225.</t>
+  </si>
+  <si>
+    <t>Grant, P.R. (1976). An 11-year study of small mammal populations at Mont St. Hilaire, Quebec. Canadian Journal of Zoology, 54, 2156–2173.</t>
+  </si>
+  <si>
+    <t>SANParks. (2004). Golden Gate Highland National Parks Census Data. South African National Park Data Repository: peggym.113.6.</t>
+  </si>
+  <si>
+    <t>SANParks. (2009). Karoo National Park Census Data. 1994 - 2009. South African National Park Data Repository: peggym.117.10.</t>
+  </si>
+  <si>
+    <t>SANParks. (1997). Census totals for large herbivores in the Kruger National Park summarized by year and region 1965-1997. South African National Park Data Repository: judithk.814.4.</t>
+  </si>
+  <si>
+    <t>Venable, D.L. (2008). Long-term population dynamics of individually mapped Sonoran Desert winter annuals from the Desert Laboratory, Tucson AZ. University of Arizona.</t>
+  </si>
+  <si>
+    <t>Adler, P.B., Tyburczy, W.R. &amp; Lauenroth, W.K. (2007). Long-term mapped quadrats from Kansas prairie: demographic information for herbaceaous plants. Ecology, 88, 2673.</t>
+  </si>
+  <si>
+    <t>Wilgers, D.J., Horne, E.A., Sandercock, B.K. &amp; Volkmann, A.W. (2006). Effects of rangeland management on community dynamics of the herpetofauna of the tallgrass prairie. Herpetologica, 62, 378–388.</t>
+  </si>
+  <si>
+    <t>Thompson, S.A. &amp; Thompson, G.G. (2005). Temporal variations in reptile assemblages in the goldfields of Western Australia. Journal of the Royal Society of Western Australia, 88, 25–36.</t>
+  </si>
+  <si>
+    <t>How, R. (1998). Long-term sampling of a herpetofaunal assemblage on an isolated urban bushland remnant, Bold Park, Perth. Journal of the Royal Society of Western Australia, 81, 143–148.</t>
+  </si>
+  <si>
+    <t>Zachmann, L., Moffet, C. &amp; Adler, P. (2010). Mapped quadrats in sagebrush steppe: long-term data for analyzing demographic rates and plant–plant interactions. Ecology, 91, 3427–3427.</t>
+  </si>
+  <si>
+    <t>Herpetofauna</t>
+  </si>
+  <si>
+    <t>Sandercock, B.K. (2009). Bird Populations. Konza Prarie LTER: CBP01. [Database].</t>
+  </si>
+  <si>
+    <t>Dickson, J.G., Conner, R.N. &amp; Williamson, J.H. (1993). Neotropical Migratory Bird Communities in a Developing Pine Plantation. 1993 Procedings on the Annual Conference. SEAFWA.</t>
+  </si>
+  <si>
+    <t>Gaston, K.J. &amp; Blackburn, T.M. (Eds.). (2007). Appendix II: Eastern Wood Breeding Bird Data. In: Pattern and Process in Macroecology. Blackwell Science Ltd, pp. 355–357.</t>
+  </si>
+  <si>
+    <t>Sauer, J.R., Hines, J.E., Gough, G., Thomas, I. &amp; Peterjohn, B.G. (1997). The North American Breeding Bird Survey Results and Analysis. Version 96.4. Patuxent Wildlife Research Center, Laurel, MD.</t>
+  </si>
+  <si>
+    <t>Mountain Bird Watch. (2010). . Vermont Center for Ecostudies.</t>
+  </si>
+  <si>
+    <t>Robert B. Waide. (2012). Avian populations Long-Term Monitoring. Luquillo LTER project of the Institute for Tropical Ecosystem Studies: Bird abundance - point counts [Database].</t>
+  </si>
+  <si>
+    <t>Henderson, P. (2010). The marine community at Hinkley Point. The Global Population Dynamics Database Version 2. NERC Centre for Population Biology, Imperial College.</t>
+  </si>
+  <si>
+    <t>Heessen, H.J.L. (1996). Time-series data for a selection of forty fish species caught during the International Bottom Trawl Survey. ICES J. Mar. Sci., 53, 1079–1084.</t>
+  </si>
+  <si>
+    <t>Time Series Length</t>
+  </si>
+  <si>
+    <t>Effect Size</t>
+  </si>
+  <si>
+    <t>Randomized Pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -716,9 +1052,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,7 +3690,7 @@
         <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C78">
         <v>83</v>
@@ -3771,10 +4116,13 @@
   <dimension ref="A1:A90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4700,8 +5048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4728,16 +5076,16 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>192</v>
+        <v>271</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>272</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>273</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4763,16 +5111,17 @@
         <v>42</v>
       </c>
       <c r="G2">
-        <v>1.6607331890000001</v>
+        <f>H2/I2</f>
+        <v>1.4608483453672492</v>
       </c>
       <c r="H2">
-        <v>-1.5386</v>
+        <v>-0.97768921860767899</v>
       </c>
       <c r="I2">
-        <v>-0.92645999999999995</v>
+        <v>-0.66926126980134504</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>4.1999999999999997E-3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4795,16 +5144,17 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>1.3196244770000001</v>
+        <f t="shared" ref="G3:G66" si="0">H3/I3</f>
+        <v>1.3002204389873377</v>
       </c>
       <c r="H3">
-        <v>-1.3063</v>
+        <v>-1.07174997144502</v>
       </c>
       <c r="I3">
-        <v>-0.9899</v>
+        <v>-0.82428328251764804</v>
       </c>
       <c r="J3">
-        <v>6.7999999999999996E-3</v>
+        <v>1.34E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4827,16 +5177,17 @@
         <v>26</v>
       </c>
       <c r="G4">
-        <v>1.6820728220000001</v>
+        <f t="shared" si="0"/>
+        <v>1.7540844557437389</v>
       </c>
       <c r="H4">
-        <v>-1.50023</v>
+        <v>-1.38287275876702</v>
       </c>
       <c r="I4">
-        <v>-0.89190000000000003</v>
-      </c>
-      <c r="J4" s="1">
-        <v>8.0000000000000004E-4</v>
+        <v>-0.78837296245275501</v>
+      </c>
+      <c r="J4">
+        <v>2.8E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4859,16 +5210,17 @@
         <v>52</v>
       </c>
       <c r="G5">
-        <v>1.3600901590000001</v>
+        <f t="shared" si="0"/>
+        <v>2.051291860667273</v>
       </c>
       <c r="H5">
-        <v>-1.5992900000000001</v>
+        <v>-2.3604758319554899</v>
       </c>
       <c r="I5">
-        <v>-1.17587</v>
+        <v>-1.1507264652177001</v>
       </c>
       <c r="J5">
-        <v>0.1132</v>
+        <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4876,7 +5228,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
         <v>106</v>
@@ -4891,16 +5243,17 @@
         <v>29</v>
       </c>
       <c r="G6">
-        <v>1.251050684</v>
+        <f t="shared" si="0"/>
+        <v>1.5982028421786405</v>
       </c>
       <c r="H6">
-        <v>-1.1455</v>
+        <v>-2.24368943204898</v>
       </c>
       <c r="I6">
-        <v>-0.91563000000000005</v>
+        <v>-1.4038827693426099</v>
       </c>
       <c r="J6">
-        <v>0.25940000000000002</v>
+        <v>0.1542</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4908,7 +5261,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -4923,16 +5276,17 @@
         <v>29</v>
       </c>
       <c r="G7">
-        <v>0.96755886099999999</v>
+        <f t="shared" si="0"/>
+        <v>1.0036720941620607</v>
       </c>
       <c r="H7">
-        <v>-0.93511</v>
+        <v>-1.21534685539328</v>
       </c>
       <c r="I7">
-        <v>-0.96645999999999999</v>
+        <v>-1.2109003154142099</v>
       </c>
       <c r="J7">
-        <v>0.69020000000000004</v>
+        <v>0.45579999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -4955,16 +5309,17 @@
         <v>16</v>
       </c>
       <c r="G8">
-        <v>1.6587816980000001</v>
+        <f t="shared" si="0"/>
+        <v>1.956490047541005</v>
       </c>
       <c r="H8">
-        <v>-1.3217399999999999</v>
+        <v>-1.01527616207996</v>
       </c>
       <c r="I8">
-        <v>-0.79681000000000002</v>
+        <v>-0.51892733283054504</v>
       </c>
       <c r="J8">
-        <v>3.2000000000000001E-2</v>
+        <v>2.3400000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4987,16 +5342,17 @@
         <v>31</v>
       </c>
       <c r="G9">
-        <v>1.1817389119999999</v>
+        <f t="shared" si="0"/>
+        <v>1.190082213344188</v>
       </c>
       <c r="H9">
-        <v>-1.04678</v>
+        <v>-0.82631459936267004</v>
       </c>
       <c r="I9">
-        <v>-0.88578999999999997</v>
+        <v>-0.69433404692326794</v>
       </c>
       <c r="J9">
-        <v>2.76E-2</v>
+        <v>3.5200000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5019,16 +5375,17 @@
         <v>9</v>
       </c>
       <c r="G10">
-        <v>1.022982316</v>
+        <f t="shared" si="0"/>
+        <v>1.0704939009546544</v>
       </c>
       <c r="H10">
-        <v>-1.01502</v>
+        <v>-3.8692197483789998</v>
       </c>
       <c r="I10">
-        <v>-0.99221999999999999</v>
+        <v>-3.61442484158805</v>
       </c>
       <c r="J10">
-        <v>0.41520000000000001</v>
+        <v>0.21779999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5051,16 +5408,17 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <v>1.1207190250000001</v>
+        <f t="shared" si="0"/>
+        <v>1.0565986216370717</v>
       </c>
       <c r="H11">
-        <v>-0.98673999999999995</v>
+        <v>-0.84097877568421198</v>
       </c>
       <c r="I11">
-        <v>-0.88044999999999995</v>
+        <v>-0.79593022218902498</v>
       </c>
       <c r="J11">
-        <v>0.40139999999999998</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5083,16 +5441,17 @@
         <v>11</v>
       </c>
       <c r="G12">
-        <v>1.0390563690000001</v>
+        <f t="shared" si="0"/>
+        <v>1.193978163004916</v>
       </c>
       <c r="H12">
-        <v>-1.0491999999999999</v>
+        <v>-1.9021986267525499</v>
       </c>
       <c r="I12">
-        <v>-1.0097700000000001</v>
+        <v>-1.5931603153991001</v>
       </c>
       <c r="J12">
-        <v>0.44740000000000002</v>
+        <v>0.1968</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5115,16 +5474,17 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <v>0.58724818400000001</v>
+        <f t="shared" si="0"/>
+        <v>0.77986514478870328</v>
       </c>
       <c r="H13">
-        <v>-0.52886999999999995</v>
+        <v>-1.4543601711110801</v>
       </c>
       <c r="I13">
-        <v>-0.90059</v>
+        <v>-1.8648867446244499</v>
       </c>
       <c r="J13">
-        <v>0.98340000000000005</v>
+        <v>0.90259999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5147,16 +5507,17 @@
         <v>11</v>
       </c>
       <c r="G14">
-        <v>1.6128184619999999</v>
+        <f t="shared" si="0"/>
+        <v>1.7626178193190301</v>
       </c>
       <c r="H14">
-        <v>-1.3597600000000001</v>
+        <v>-2.8935353146794101</v>
       </c>
       <c r="I14">
-        <v>-0.84309999999999996</v>
-      </c>
-      <c r="J14" s="1">
-        <v>4.0000000000000002E-4</v>
+        <v>-1.6416124261113501</v>
+      </c>
+      <c r="J14">
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5164,7 +5525,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
         <v>104</v>
@@ -5179,16 +5540,17 @@
         <v>20</v>
       </c>
       <c r="G15">
-        <v>1.290705335</v>
+        <f t="shared" si="0"/>
+        <v>1.1774388955800994</v>
       </c>
       <c r="H15">
-        <v>-1.1364700000000001</v>
+        <v>-1.4993175362170601</v>
       </c>
       <c r="I15">
-        <v>-0.88049999999999995</v>
+        <v>-1.2733718427726799</v>
       </c>
       <c r="J15">
-        <v>7.1800000000000003E-2</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5196,7 +5558,7 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>113</v>
@@ -5211,16 +5573,17 @@
         <v>17</v>
       </c>
       <c r="G16">
-        <v>1.318040627</v>
+        <f t="shared" si="0"/>
+        <v>1.9719884009687021</v>
       </c>
       <c r="H16">
-        <v>-1.30453</v>
+        <v>-4.9015839612245902</v>
       </c>
       <c r="I16">
-        <v>-0.98975000000000002</v>
+        <v>-2.4856048640127799</v>
       </c>
       <c r="J16">
-        <v>5.7000000000000002E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5228,10 +5591,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D17">
         <v>14</v>
@@ -5243,16 +5606,17 @@
         <v>17</v>
       </c>
       <c r="G17">
-        <v>1.1778721000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.2894055156150801</v>
       </c>
       <c r="H17">
-        <v>-0.98443999999999998</v>
+        <v>-3.8663844395697899</v>
       </c>
       <c r="I17">
-        <v>-0.83577999999999997</v>
+        <v>-2.9985791069967802</v>
       </c>
       <c r="J17">
-        <v>8.6199999999999999E-2</v>
+        <v>3.0599999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5260,10 +5624,10 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D18">
         <v>7</v>
@@ -5275,16 +5639,17 @@
         <v>24</v>
       </c>
       <c r="G18">
-        <v>1.6508143179999999</v>
+        <f t="shared" si="0"/>
+        <v>1.8054804171424808</v>
       </c>
       <c r="H18">
-        <v>-0.93391000000000002</v>
+        <v>-2.68337474816511</v>
       </c>
       <c r="I18">
-        <v>-0.56572999999999996</v>
+        <v>-1.4862386335998401</v>
       </c>
       <c r="J18">
-        <v>1.2200000000000001E-2</v>
+        <v>1.4800000000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -5292,7 +5657,7 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
         <v>113</v>
@@ -5307,16 +5672,17 @@
         <v>24</v>
       </c>
       <c r="G19">
-        <v>1.027822013</v>
+        <f t="shared" si="0"/>
+        <v>1.0849854696596684</v>
       </c>
       <c r="H19">
-        <v>-0.79795000000000005</v>
+        <v>-3.4012183111151399</v>
       </c>
       <c r="I19">
-        <v>-0.77634999999999998</v>
+        <v>-3.1348054017553002</v>
       </c>
       <c r="J19">
-        <v>0.46100000000000002</v>
+        <v>0.31480000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5324,7 +5690,7 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
         <v>114</v>
@@ -5339,16 +5705,17 @@
         <v>24</v>
       </c>
       <c r="G20">
-        <v>1.0222279439999999</v>
+        <f t="shared" si="0"/>
+        <v>1.0472896856350435</v>
       </c>
       <c r="H20">
-        <v>-0.96211000000000002</v>
+        <v>-12.474625429478399</v>
       </c>
       <c r="I20">
-        <v>-0.94118999999999997</v>
+        <v>-11.911341819349801</v>
       </c>
       <c r="J20">
-        <v>0.3604</v>
+        <v>0.20880000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5356,7 +5723,7 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
         <v>117</v>
@@ -5371,24 +5738,25 @@
         <v>24</v>
       </c>
       <c r="G21">
-        <v>2.6485758019999999</v>
+        <f t="shared" si="0"/>
+        <v>1.1925822166120412</v>
       </c>
       <c r="H21">
-        <v>-1.0565</v>
+        <v>-26.7981247309033</v>
       </c>
       <c r="I21">
-        <v>-0.39889000000000002</v>
+        <v>-22.4706727616927</v>
       </c>
       <c r="J21">
-        <v>1.9800000000000002E-2</v>
+        <v>0.1532</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
         <v>118</v>
@@ -5403,21 +5771,22 @@
         <v>4</v>
       </c>
       <c r="G22">
-        <v>-1.9814685139999999</v>
+        <f t="shared" si="0"/>
+        <v>-1.4188131199752358</v>
       </c>
       <c r="H22">
-        <v>0.28337499999999999</v>
+        <v>0.115496284724391</v>
       </c>
       <c r="I22">
-        <v>-0.14301</v>
+        <v>-8.1403451306121893E-2</v>
       </c>
       <c r="J22">
-        <v>0.75560000000000005</v>
+        <v>0.68799999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s">
         <v>119</v>
@@ -5435,21 +5804,22 @@
         <v>7</v>
       </c>
       <c r="G23">
-        <v>2.0104242210000001</v>
+        <f t="shared" si="0"/>
+        <v>0.25327762727863978</v>
       </c>
       <c r="H23">
-        <v>-0.84772000000000003</v>
+        <v>-6.1542829187137403E-2</v>
       </c>
       <c r="I23">
-        <v>-0.42165999999999998</v>
+        <v>-0.242985651154383</v>
       </c>
       <c r="J23">
-        <v>0.29699999999999999</v>
+        <v>0.66139999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
         <v>119</v>
@@ -5467,21 +5837,22 @@
         <v>7</v>
       </c>
       <c r="G24">
-        <v>1.050686292</v>
+        <f t="shared" si="0"/>
+        <v>0.71333827910916014</v>
       </c>
       <c r="H24">
-        <v>-0.85163</v>
+        <v>-0.69902470338260703</v>
       </c>
       <c r="I24">
-        <v>-0.81054999999999999</v>
+        <v>-0.97993437875725897</v>
       </c>
       <c r="J24">
-        <v>0.45960000000000001</v>
+        <v>0.8236</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B25" t="s">
         <v>122</v>
@@ -5499,21 +5870,22 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>0.86245804000000004</v>
+        <f t="shared" si="0"/>
+        <v>1.1375601895687504</v>
       </c>
       <c r="H25">
-        <v>-0.69808999999999999</v>
+        <v>-1.2604878376303901</v>
       </c>
       <c r="I25">
-        <v>-0.80942000000000003</v>
+        <v>-1.10806254402085</v>
       </c>
       <c r="J25">
-        <v>0.64580000000000004</v>
+        <v>0.30620000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s">
         <v>122</v>
@@ -5531,24 +5903,25 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>0.57183327399999995</v>
+        <f t="shared" si="0"/>
+        <v>0.71305163152624962</v>
       </c>
       <c r="H26">
-        <v>-0.25063999999999997</v>
+        <v>-0.16253846453628301</v>
       </c>
       <c r="I26">
-        <v>-0.43830999999999998</v>
+        <v>-0.22794767917209299</v>
       </c>
       <c r="J26">
-        <v>0.63119999999999998</v>
+        <v>0.55720000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B27" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C27" t="s">
         <v>120</v>
@@ -5563,24 +5936,25 @@
         <v>4</v>
       </c>
       <c r="G27">
-        <v>-1.271569891</v>
+        <f t="shared" si="0"/>
+        <v>-1.4271463304230325</v>
       </c>
       <c r="H27">
-        <v>1.0735870000000001</v>
+        <v>0.96980224213541799</v>
       </c>
       <c r="I27">
-        <v>-0.84430000000000005</v>
+        <v>-0.67953945678993599</v>
       </c>
       <c r="J27">
-        <v>0.99639999999999995</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C28" t="s">
         <v>121</v>
@@ -5595,24 +5969,25 @@
         <v>4</v>
       </c>
       <c r="G28">
-        <v>0.73121665700000005</v>
+        <f t="shared" si="0"/>
+        <v>0.90733169305382444</v>
       </c>
       <c r="H28">
-        <v>-0.65251000000000003</v>
+        <v>-0.90224163533657598</v>
       </c>
       <c r="I28">
-        <v>-0.89237</v>
+        <v>-0.994390080544727</v>
       </c>
       <c r="J28">
-        <v>0.88300000000000001</v>
+        <v>0.67859999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C29" t="s">
         <v>120</v>
@@ -5627,24 +6002,25 @@
         <v>58</v>
       </c>
       <c r="G29">
-        <v>0.32697746700000002</v>
+        <f t="shared" si="0"/>
+        <v>0.24047425037632278</v>
       </c>
       <c r="H29">
-        <v>-0.17995</v>
+        <v>-2.0433546386164299E-2</v>
       </c>
       <c r="I29">
-        <v>-0.55035000000000001</v>
+        <v>-8.4971868523084901E-2</v>
       </c>
       <c r="J29">
-        <v>0.72440000000000004</v>
+        <v>0.745</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C30" t="s">
         <v>126</v>
@@ -5659,24 +6035,25 @@
         <v>15</v>
       </c>
       <c r="G30">
-        <v>0.63157659300000002</v>
+        <f t="shared" si="0"/>
+        <v>0.64090073836279227</v>
       </c>
       <c r="H30">
-        <v>-0.62456999999999996</v>
+        <v>-0.27562727132561698</v>
       </c>
       <c r="I30">
-        <v>-0.9889</v>
+        <v>-0.43006234012105898</v>
       </c>
       <c r="J30">
-        <v>0.86360000000000003</v>
+        <v>0.84940000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C31" t="s">
         <v>128</v>
@@ -5691,21 +6068,22 @@
         <v>18</v>
       </c>
       <c r="G31">
-        <v>-2.6088434409999999</v>
+        <f t="shared" si="0"/>
+        <v>-8.0635151021552134E-3</v>
       </c>
       <c r="H31">
-        <v>1.0229710000000001</v>
+        <v>5.8054075574932498E-3</v>
       </c>
       <c r="I31">
-        <v>-0.39212000000000002</v>
+        <v>-0.71995990383171504</v>
       </c>
       <c r="J31">
-        <v>0.93959999999999999</v>
+        <v>0.91739999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s">
         <v>129</v>
@@ -5723,16 +6101,17 @@
         <v>16</v>
       </c>
       <c r="G32">
-        <v>0.93387449499999997</v>
+        <f t="shared" si="0"/>
+        <v>1.2525801782462826</v>
       </c>
       <c r="H32">
-        <v>-0.82294999999999996</v>
+        <v>-2.2253953850655899</v>
       </c>
       <c r="I32">
-        <v>-0.88122</v>
+        <v>-1.7766490510662001</v>
       </c>
       <c r="J32">
-        <v>0.75139999999999996</v>
+        <v>2.92E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -5755,16 +6134,17 @@
         <v>66</v>
       </c>
       <c r="G33">
-        <v>1.05022054</v>
+        <f t="shared" si="0"/>
+        <v>7.2697743387034983E-2</v>
       </c>
       <c r="H33">
-        <v>-0.74578999999999995</v>
+        <v>-0.303405642564676</v>
       </c>
       <c r="I33">
-        <v>-0.71013000000000004</v>
+        <v>-4.1735221539047904</v>
       </c>
       <c r="J33">
-        <v>0.55520000000000003</v>
+        <v>0.86240000000000006</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -5787,16 +6167,17 @@
         <v>12</v>
       </c>
       <c r="G34">
-        <v>3.308495824</v>
+        <f t="shared" si="0"/>
+        <v>3.2270555496652578</v>
       </c>
       <c r="H34">
-        <v>-1.7713000000000001</v>
+        <v>-2.2806763038634998</v>
       </c>
       <c r="I34">
-        <v>-0.53537999999999997</v>
-      </c>
-      <c r="J34" s="1">
-        <v>2.0000000000000001E-4</v>
+        <v>-0.70673599160698497</v>
+      </c>
+      <c r="J34">
+        <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -5804,7 +6185,7 @@
         <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C35" t="s">
         <v>135</v>
@@ -5819,16 +6200,17 @@
         <v>6</v>
       </c>
       <c r="G35">
-        <v>1.3860094970000001</v>
+        <f t="shared" si="0"/>
+        <v>2.1023798340250139</v>
       </c>
       <c r="H35">
-        <v>-1.01329</v>
+        <v>-0.72949459797873595</v>
       </c>
       <c r="I35">
-        <v>-0.73107999999999995</v>
+        <v>-0.34698515756884701</v>
       </c>
       <c r="J35">
-        <v>0.28339999999999999</v>
+        <v>9.6600000000000005E-2</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -5836,7 +6218,7 @@
         <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
         <v>137</v>
@@ -5851,16 +6233,17 @@
         <v>6</v>
       </c>
       <c r="G36">
-        <v>0.14395702399999999</v>
+        <f t="shared" si="0"/>
+        <v>0.23427273211528465</v>
       </c>
       <c r="H36">
-        <v>-0.10052</v>
+        <v>-0.15983736274312099</v>
       </c>
       <c r="I36">
-        <v>-0.69828000000000001</v>
+        <v>-0.68227045162245203</v>
       </c>
       <c r="J36">
-        <v>0.95399999999999996</v>
+        <v>0.93559999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -5868,7 +6251,7 @@
         <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
         <v>139</v>
@@ -5883,16 +6266,17 @@
         <v>6</v>
       </c>
       <c r="G37">
-        <v>0.40472417199999999</v>
+        <f t="shared" si="0"/>
+        <v>1.604362973405407</v>
       </c>
       <c r="H37">
-        <v>-0.28314</v>
+        <v>-0.30768160951794499</v>
       </c>
       <c r="I37">
-        <v>-0.69959000000000005</v>
+        <v>-0.19177805435441</v>
       </c>
       <c r="J37">
-        <v>0.6462</v>
+        <v>0.2702</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -5900,7 +6284,7 @@
         <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
         <v>141</v>
@@ -5915,16 +6299,17 @@
         <v>6</v>
       </c>
       <c r="G38">
-        <v>1.981104671</v>
+        <f t="shared" si="0"/>
+        <v>3.2381045268485682</v>
       </c>
       <c r="H38">
-        <v>-1.32673</v>
+        <v>-1.1615056613713499</v>
       </c>
       <c r="I38">
-        <v>-0.66969000000000001</v>
+        <v>-0.35869924881695098</v>
       </c>
       <c r="J38">
-        <v>0.1174</v>
+        <v>2.5399999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -5932,7 +6317,7 @@
         <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C39" t="s">
         <v>142</v>
@@ -5947,16 +6332,17 @@
         <v>17</v>
       </c>
       <c r="G39">
-        <v>1.14288615</v>
+        <f t="shared" si="0"/>
+        <v>1.276792911914133</v>
       </c>
       <c r="H39">
-        <v>-0.91732000000000002</v>
+        <v>-2.4930138551290302</v>
       </c>
       <c r="I39">
-        <v>-0.80262999999999995</v>
+        <v>-1.95255928495998</v>
       </c>
       <c r="J39">
-        <v>7.2800000000000004E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -5979,16 +6365,17 @@
         <v>32</v>
       </c>
       <c r="G40">
-        <v>0.85972694100000002</v>
+        <f t="shared" si="0"/>
+        <v>1.019407004810764</v>
       </c>
       <c r="H40">
-        <v>-0.79920999999999998</v>
+        <v>-3.2288033034994101</v>
       </c>
       <c r="I40">
-        <v>-0.92961000000000005</v>
+        <v>-3.1673348213835202</v>
       </c>
       <c r="J40">
-        <v>0.90380000000000005</v>
+        <v>0.43680000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -6011,16 +6398,17 @@
         <v>11</v>
       </c>
       <c r="G41">
-        <v>1.972430371</v>
+        <f t="shared" si="0"/>
+        <v>1.2226850050374793</v>
       </c>
       <c r="H41">
-        <v>-1.81528</v>
+        <v>-0.20150209253088799</v>
       </c>
       <c r="I41">
-        <v>-0.92032999999999998</v>
+        <v>-0.16480294736640799</v>
       </c>
       <c r="J41">
-        <v>0.29320000000000002</v>
+        <v>0.34560000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -6043,16 +6431,17 @@
         <v>11</v>
       </c>
       <c r="G42">
-        <v>4.3910415049999996</v>
+        <f t="shared" si="0"/>
+        <v>1.1290875927864363</v>
       </c>
       <c r="H42">
-        <v>-0.97035000000000005</v>
+        <v>-5.4033297401407703</v>
       </c>
       <c r="I42">
-        <v>-0.22098999999999999</v>
+        <v>-4.7855717967868898</v>
       </c>
       <c r="J42">
-        <v>0.70179999999999998</v>
+        <v>0.45300000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -6075,16 +6464,17 @@
         <v>11</v>
       </c>
       <c r="G43">
-        <v>1.2268269060000001</v>
+        <f t="shared" si="0"/>
+        <v>1.7721848987025242</v>
       </c>
       <c r="H43">
-        <v>-0.93432999999999999</v>
+        <v>-8.3982636860462705</v>
       </c>
       <c r="I43">
-        <v>-0.76158000000000003</v>
+        <v>-4.7389319772417204</v>
       </c>
       <c r="J43">
-        <v>0.24679999999999999</v>
+        <v>7.3400000000000007E-2</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -6107,16 +6497,17 @@
         <v>11</v>
       </c>
       <c r="G44">
-        <v>0.95931096999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.0291301791465877</v>
       </c>
       <c r="H44">
-        <v>-0.68250999999999995</v>
+        <v>-4.1778586498479502</v>
       </c>
       <c r="I44">
-        <v>-0.71145999999999998</v>
+        <v>-4.0596017243537297</v>
       </c>
       <c r="J44">
-        <v>0.5756</v>
+        <v>0.44119999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -6139,16 +6530,17 @@
         <v>11</v>
       </c>
       <c r="G45">
-        <v>1.4513466930000001</v>
+        <f t="shared" si="0"/>
+        <v>2.1927565562026956</v>
       </c>
       <c r="H45">
-        <v>-0.96494999999999997</v>
+        <v>-8.4163957907250797</v>
       </c>
       <c r="I45">
-        <v>-0.66486000000000001</v>
+        <v>-3.8382718623813701</v>
       </c>
       <c r="J45">
-        <v>0.2472</v>
+        <v>0.1026</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -6171,16 +6563,17 @@
         <v>11</v>
       </c>
       <c r="G46">
-        <v>1.3262230909999999</v>
+        <f t="shared" si="0"/>
+        <v>1.641517080527152</v>
       </c>
       <c r="H46">
-        <v>-0.87478999999999996</v>
+        <v>-10.2167526905932</v>
       </c>
       <c r="I46">
-        <v>-0.65961000000000003</v>
+        <v>-6.2239697727130698</v>
       </c>
       <c r="J46">
-        <v>0.21820000000000001</v>
+        <v>0.12920000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -6203,16 +6596,17 @@
         <v>11</v>
       </c>
       <c r="G47">
-        <v>0.68730047100000002</v>
+        <f t="shared" si="0"/>
+        <v>0.61126871029673069</v>
       </c>
       <c r="H47">
-        <v>-0.52498999999999996</v>
+        <v>-4.0001623574233696</v>
       </c>
       <c r="I47">
-        <v>-0.76383999999999996</v>
+        <v>-6.5440325834469002</v>
       </c>
       <c r="J47">
-        <v>0.71199999999999997</v>
+        <v>0.56599999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -6235,16 +6629,17 @@
         <v>11</v>
       </c>
       <c r="G48">
-        <v>1.6582451499999999</v>
+        <f t="shared" si="0"/>
+        <v>1.6066984913387639</v>
       </c>
       <c r="H48">
-        <v>-0.94416999999999995</v>
+        <v>-8.2473972445595294</v>
       </c>
       <c r="I48">
-        <v>-0.56938</v>
+        <v>-5.1331331229965098</v>
       </c>
       <c r="J48">
-        <v>0.1646</v>
+        <v>0.23719999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -6267,16 +6662,17 @@
         <v>11</v>
       </c>
       <c r="G49">
-        <v>1.117567765</v>
+        <f t="shared" si="0"/>
+        <v>0.98747820974810041</v>
       </c>
       <c r="H49">
-        <v>-0.78998000000000002</v>
+        <v>-6.4024926204700998</v>
       </c>
       <c r="I49">
-        <v>-0.70687</v>
+        <v>-6.4836799002413796</v>
       </c>
       <c r="J49">
-        <v>0.45079999999999998</v>
+        <v>0.49120000000000003</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -6299,16 +6695,17 @@
         <v>11</v>
       </c>
       <c r="G50">
-        <v>2.864841733</v>
+        <f t="shared" si="0"/>
+        <v>2.212749408490323</v>
       </c>
       <c r="H50">
-        <v>-1.2565</v>
+        <v>-9.8484615904100803</v>
       </c>
       <c r="I50">
-        <v>-0.43858999999999998</v>
+        <v>-4.4507803516392404</v>
       </c>
       <c r="J50">
-        <v>5.5800000000000002E-2</v>
+        <v>0.1482</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -6331,16 +6728,17 @@
         <v>11</v>
       </c>
       <c r="G51">
-        <v>0.77233574999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.96796500094863736</v>
       </c>
       <c r="H51">
-        <v>-0.61873999999999996</v>
+        <v>-5.8119804677754896</v>
       </c>
       <c r="I51">
-        <v>-0.80112000000000005</v>
+        <v>-6.0043291462806598</v>
       </c>
       <c r="J51">
-        <v>0.83040000000000003</v>
+        <v>0.51080000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -6363,16 +6761,17 @@
         <v>10</v>
       </c>
       <c r="G52">
-        <v>1.736952775</v>
+        <f t="shared" si="0"/>
+        <v>1.6855839049020696</v>
       </c>
       <c r="H52">
-        <v>-1.33646</v>
+        <v>-1.6459488181591999</v>
       </c>
       <c r="I52">
-        <v>-0.76942999999999995</v>
+        <v>-0.97648584171479003</v>
       </c>
       <c r="J52">
-        <v>2E-3</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -6395,16 +6794,17 @@
         <v>10</v>
       </c>
       <c r="G53">
-        <v>1.567901344</v>
+        <f t="shared" si="0"/>
+        <v>2.0278884449994017</v>
       </c>
       <c r="H53">
-        <v>-1.2628999999999999</v>
+        <v>-2.3981745283733802</v>
       </c>
       <c r="I53">
-        <v>-0.80547000000000002</v>
-      </c>
-      <c r="J53">
-        <v>2.3999999999999998E-3</v>
+        <v>-1.18259687029978</v>
+      </c>
+      <c r="J53" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -6427,16 +6827,17 @@
         <v>10</v>
       </c>
       <c r="G54">
-        <v>1.082967099</v>
+        <f t="shared" si="0"/>
+        <v>2.3121549832932398</v>
       </c>
       <c r="H54">
-        <v>-1.0152399999999999</v>
+        <v>-3.4648234382384899</v>
       </c>
       <c r="I54">
-        <v>-0.93745999999999996</v>
-      </c>
-      <c r="J54">
-        <v>0.29099999999999998</v>
+        <v>-1.4985256019920801</v>
+      </c>
+      <c r="J54" s="1">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -6459,16 +6860,17 @@
         <v>10</v>
       </c>
       <c r="G55">
-        <v>1.2078837570000001</v>
+        <f t="shared" si="0"/>
+        <v>1.337836740341277</v>
       </c>
       <c r="H55">
-        <v>-1.0751999999999999</v>
+        <v>-2.1599644091338899</v>
       </c>
       <c r="I55">
-        <v>-0.89015</v>
+        <v>-1.6145201757449801</v>
       </c>
       <c r="J55">
-        <v>1.2200000000000001E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -6491,16 +6893,17 @@
         <v>10</v>
       </c>
       <c r="G56">
-        <v>1.4955217999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.6025308989971145</v>
       </c>
       <c r="H56">
-        <v>-1.24614</v>
+        <v>-1.9129008092514901</v>
       </c>
       <c r="I56">
-        <v>-0.83323999999999998</v>
+        <v>-1.1936748367526699</v>
       </c>
       <c r="J56">
-        <v>4.7999999999999996E-3</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -6523,16 +6926,17 @@
         <v>10</v>
       </c>
       <c r="G57">
-        <v>1.9847524059999999</v>
+        <f t="shared" si="0"/>
+        <v>5.0984648803623323</v>
       </c>
       <c r="H57">
-        <v>-1.39907</v>
+        <v>-3.22523676960768</v>
       </c>
       <c r="I57">
-        <v>-0.70491000000000004</v>
+        <v>-0.63258977854888598</v>
       </c>
       <c r="J57">
-        <v>1.4200000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -6555,16 +6959,17 @@
         <v>22</v>
       </c>
       <c r="G58">
-        <v>2.515926146</v>
+        <f t="shared" si="0"/>
+        <v>2.5366463758984525</v>
       </c>
       <c r="H58">
-        <v>-1.4880500000000001</v>
+        <v>-1.16791765539929</v>
       </c>
       <c r="I58">
-        <v>-0.59145000000000003</v>
-      </c>
-      <c r="J58" s="1">
-        <v>5.9999999999999995E-4</v>
+        <v>-0.46041800169549701</v>
+      </c>
+      <c r="J58">
+        <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -6572,7 +6977,7 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C59" t="s">
         <v>164</v>
@@ -6587,16 +6992,17 @@
         <v>17</v>
       </c>
       <c r="G59">
-        <v>1.749514215</v>
+        <f t="shared" si="0"/>
+        <v>3.0034112540512754</v>
       </c>
       <c r="H59">
-        <v>-1.0837000000000001</v>
+        <v>-2.3576986452291799</v>
       </c>
       <c r="I59">
-        <v>-0.61943000000000004</v>
+        <v>-0.785006929054055</v>
       </c>
       <c r="J59">
-        <v>0.19900000000000001</v>
+        <v>1.44E-2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -6604,7 +7010,7 @@
         <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
         <v>164</v>
@@ -6619,16 +7025,17 @@
         <v>17</v>
       </c>
       <c r="G60">
-        <v>1.7887678549999999</v>
+        <f t="shared" si="0"/>
+        <v>1.6435140317855867</v>
       </c>
       <c r="H60">
-        <v>-1.4022699999999999</v>
+        <v>-1.9772705713627701</v>
       </c>
       <c r="I60">
-        <v>-0.78393000000000002</v>
+        <v>-1.2030749559312099</v>
       </c>
       <c r="J60">
-        <v>1.4E-2</v>
+        <v>4.36E-2</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -6636,7 +7043,7 @@
         <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C61" t="s">
         <v>164</v>
@@ -6651,16 +7058,17 @@
         <v>17</v>
       </c>
       <c r="G61">
-        <v>1.4496867360000001</v>
+        <f t="shared" si="0"/>
+        <v>1.4212077449270371</v>
       </c>
       <c r="H61">
-        <v>-1.1371500000000001</v>
+        <v>-0.96006332089000002</v>
       </c>
       <c r="I61">
-        <v>-0.78441000000000005</v>
+        <v>-0.67552637840380503</v>
       </c>
       <c r="J61">
-        <v>8.2000000000000003E-2</v>
+        <v>9.7799999999999998E-2</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -6668,7 +7076,7 @@
         <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C62" t="s">
         <v>164</v>
@@ -6683,16 +7091,17 @@
         <v>17</v>
       </c>
       <c r="G62">
-        <v>2.6258796480000002</v>
+        <f t="shared" si="0"/>
+        <v>7.5002624428272364</v>
       </c>
       <c r="H62">
-        <v>-2.0425</v>
+        <v>-1.31289739694991</v>
       </c>
       <c r="I62">
-        <v>-0.77783000000000002</v>
+        <v>-0.17504686095424299</v>
       </c>
       <c r="J62">
-        <v>8.2199999999999995E-2</v>
+        <v>2.5999999999999999E-3</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -6715,16 +7124,17 @@
         <v>14</v>
       </c>
       <c r="G63">
-        <v>1.0594443360000001</v>
+        <f t="shared" si="0"/>
+        <v>1.0947337885130639</v>
       </c>
       <c r="H63">
-        <v>-0.68689999999999996</v>
+        <v>-1.2732637029701599</v>
       </c>
       <c r="I63">
-        <v>-0.64836000000000005</v>
+        <v>-1.1630806652086501</v>
       </c>
       <c r="J63">
-        <v>0.41720000000000002</v>
+        <v>0.3624</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -6747,16 +7157,17 @@
         <v>12</v>
       </c>
       <c r="G64">
-        <v>1.490726258</v>
+        <f t="shared" si="0"/>
+        <v>1.0783662922864068</v>
       </c>
       <c r="H64">
-        <v>-0.37497000000000003</v>
+        <v>-1.3462743716325201</v>
       </c>
       <c r="I64">
-        <v>-0.25152999999999998</v>
+        <v>-1.24843884797074</v>
       </c>
       <c r="J64">
-        <v>0.435</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -6764,7 +7175,7 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C65" t="s">
         <v>164</v>
@@ -6779,16 +7190,17 @@
         <v>13</v>
       </c>
       <c r="G65">
-        <v>3.5149482129999998</v>
+        <f t="shared" si="0"/>
+        <v>3.2077934106400514</v>
       </c>
       <c r="H65">
-        <v>-0.41979</v>
+        <v>-0.60941311825123201</v>
       </c>
       <c r="I65">
-        <v>-0.11942999999999999</v>
+        <v>-0.189978917043051</v>
       </c>
       <c r="J65">
-        <v>0.21920000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -6796,7 +7208,7 @@
         <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C66" t="s">
         <v>164</v>
@@ -6811,16 +7223,17 @@
         <v>13</v>
       </c>
       <c r="G66">
-        <v>0.86288690999999995</v>
+        <f t="shared" si="0"/>
+        <v>0.13394261654727496</v>
       </c>
       <c r="H66">
-        <v>-0.75846999999999998</v>
+        <v>-0.148176762780933</v>
       </c>
       <c r="I66">
-        <v>-0.879</v>
+        <v>-1.10627048060267</v>
       </c>
       <c r="J66">
-        <v>0.68359999999999999</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -6843,16 +7256,17 @@
         <v>21</v>
       </c>
       <c r="G67">
-        <v>10.129159380000001</v>
+        <f t="shared" ref="G67:G91" si="1">H67/I67</f>
+        <v>11.581529292751259</v>
       </c>
       <c r="H67">
-        <v>-1.2090099999999999</v>
+        <v>-1.6193615077455501</v>
       </c>
       <c r="I67">
-        <v>-0.11935999999999999</v>
+        <v>-0.13982277010334801</v>
       </c>
       <c r="J67">
-        <v>1.5800000000000002E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -6875,16 +7289,17 @@
         <v>21</v>
       </c>
       <c r="G68">
-        <v>0.98108890400000004</v>
+        <f t="shared" si="1"/>
+        <v>0.90773894606791161</v>
       </c>
       <c r="H68">
-        <v>-0.73882999999999999</v>
+        <v>-1.04012604308761</v>
       </c>
       <c r="I68">
-        <v>-0.75307000000000002</v>
+        <v>-1.1458426980501</v>
       </c>
       <c r="J68">
-        <v>0.5444</v>
+        <v>0.63139999999999996</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -6907,16 +7322,17 @@
         <v>7</v>
       </c>
       <c r="G69">
-        <v>3.2373291329999998</v>
+        <f t="shared" si="1"/>
+        <v>1.7667572982396129</v>
       </c>
       <c r="H69">
-        <v>-1.62107</v>
+        <v>-3.0495597541764901</v>
       </c>
       <c r="I69">
-        <v>-0.50073999999999996</v>
+        <v>-1.7260773492856401</v>
       </c>
       <c r="J69">
-        <v>4.7399999999999998E-2</v>
+        <v>0.1358</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -6939,16 +7355,17 @@
         <v>44</v>
       </c>
       <c r="G70">
-        <v>1.214866977</v>
+        <f t="shared" si="1"/>
+        <v>1.1440432722767919</v>
       </c>
       <c r="H70">
-        <v>-0.98845000000000005</v>
+        <v>-2.7556106269764999</v>
       </c>
       <c r="I70">
-        <v>-0.81362999999999996</v>
+        <v>-2.40865943950921</v>
       </c>
       <c r="J70">
-        <v>3.9600000000000003E-2</v>
+        <v>0.17080000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -6956,7 +7373,7 @@
         <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C71" t="s">
         <v>164</v>
@@ -6971,16 +7388,17 @@
         <v>11</v>
       </c>
       <c r="G71">
-        <v>1.6988301560000001</v>
+        <f t="shared" si="1"/>
+        <v>3.306307974834048</v>
       </c>
       <c r="H71">
-        <v>-1.2256100000000001</v>
+        <v>-2.2783187574347101</v>
       </c>
       <c r="I71">
-        <v>-0.72143999999999997</v>
+        <v>-0.68908243720068596</v>
       </c>
       <c r="J71">
-        <v>9.6799999999999997E-2</v>
+        <v>1.52E-2</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -7003,16 +7421,17 @@
         <v>16</v>
       </c>
       <c r="G72">
-        <v>1.2469364780000001</v>
+        <f t="shared" si="1"/>
+        <v>1.0413913920586519</v>
       </c>
       <c r="H72">
-        <v>-1.07447</v>
+        <v>-2.1806240549094502</v>
       </c>
       <c r="I72">
-        <v>-0.86168</v>
+        <v>-2.0939524481748699</v>
       </c>
       <c r="J72">
-        <v>8.14E-2</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -7035,16 +7454,17 @@
         <v>17</v>
       </c>
       <c r="G73">
-        <v>0.37356431200000001</v>
+        <f t="shared" si="1"/>
+        <v>1.3158738259202583</v>
       </c>
       <c r="H73">
-        <v>-0.35531000000000001</v>
+        <v>-3.36298959006721</v>
       </c>
       <c r="I73">
-        <v>-0.95115000000000005</v>
+        <v>-2.5557082478749802</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -7067,16 +7487,17 @@
         <v>11</v>
       </c>
       <c r="G74">
-        <v>1.4989596160000001</v>
+        <f t="shared" si="1"/>
+        <v>2.3345988005408005</v>
       </c>
       <c r="H74">
-        <v>-1.1764300000000001</v>
+        <v>-1.4305472172893401</v>
       </c>
       <c r="I74">
-        <v>-0.78483000000000003</v>
+        <v>-0.61275933876002997</v>
       </c>
       <c r="J74">
-        <v>0.16600000000000001</v>
+        <v>4.58E-2</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -7099,16 +7520,17 @@
         <v>29</v>
       </c>
       <c r="G75">
-        <v>1.254320646</v>
+        <f t="shared" si="1"/>
+        <v>1.5327512347790464</v>
       </c>
       <c r="H75">
-        <v>-1.1366700000000001</v>
+        <v>-3.12688457470676</v>
       </c>
       <c r="I75">
-        <v>-0.90620000000000001</v>
+        <v>-2.0400470107319899</v>
       </c>
       <c r="J75">
-        <v>5.5199999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -7131,16 +7553,17 @@
         <v>21</v>
       </c>
       <c r="G76">
-        <v>1.1826389530000001</v>
+        <f t="shared" si="1"/>
+        <v>1.5258413676130052</v>
       </c>
       <c r="H76">
-        <v>-1.00573</v>
+        <v>-2.4452965409393599</v>
       </c>
       <c r="I76">
-        <v>-0.85041</v>
+        <v>-1.60258896687585</v>
       </c>
       <c r="J76">
-        <v>0.1976</v>
+        <v>3.9199999999999999E-2</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -7148,7 +7571,7 @@
         <v>101</v>
       </c>
       <c r="B77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C77" t="s">
         <v>182</v>
@@ -7163,16 +7586,17 @@
         <v>20</v>
       </c>
       <c r="G77">
-        <v>1.4948618650000001</v>
+        <f t="shared" si="1"/>
+        <v>1.6523073546804017</v>
       </c>
       <c r="H77">
-        <v>-1.2820400000000001</v>
+        <v>-3.61593508017926</v>
       </c>
       <c r="I77">
-        <v>-0.85763</v>
+        <v>-2.1884155329434298</v>
       </c>
       <c r="J77">
-        <v>1.0800000000000001E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -7180,7 +7604,7 @@
         <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C78" t="s">
         <v>183</v>
@@ -7195,16 +7619,17 @@
         <v>19</v>
       </c>
       <c r="G78">
-        <v>1.2528697390000001</v>
+        <f t="shared" si="1"/>
+        <v>1.0485274811919498</v>
       </c>
       <c r="H78">
-        <v>-0.97355000000000003</v>
+        <v>-3.0504967587632299</v>
       </c>
       <c r="I78">
-        <v>-0.77705999999999997</v>
+        <v>-2.90931502843919</v>
       </c>
       <c r="J78">
-        <v>0.16039999999999999</v>
+        <v>0.40379999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -7212,7 +7637,7 @@
         <v>101</v>
       </c>
       <c r="B79" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C79" t="s">
         <v>182</v>
@@ -7227,16 +7652,17 @@
         <v>20</v>
       </c>
       <c r="G79">
-        <v>1.097071935</v>
+        <f t="shared" si="1"/>
+        <v>0.77415673798807516</v>
       </c>
       <c r="H79">
-        <v>-0.99934999999999996</v>
+        <v>-2.7965511074225602</v>
       </c>
       <c r="I79">
-        <v>-0.91091999999999995</v>
+        <v>-3.61238360424325</v>
       </c>
       <c r="J79">
-        <v>0.18140000000000001</v>
+        <v>0.88100000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -7244,7 +7670,7 @@
         <v>101</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C80" t="s">
         <v>183</v>
@@ -7259,16 +7685,17 @@
         <v>19</v>
       </c>
       <c r="G80">
-        <v>0.97751866499999995</v>
+        <f t="shared" si="1"/>
+        <v>1.3395497016710549</v>
       </c>
       <c r="H80">
-        <v>-0.94928999999999997</v>
+        <v>-6.7017389046435802</v>
       </c>
       <c r="I80">
-        <v>-0.97111999999999998</v>
+        <v>-5.0029789087208396</v>
       </c>
       <c r="J80">
-        <v>0.62539999999999996</v>
+        <v>3.2599999999999997E-2</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -7276,7 +7703,7 @@
         <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C81" t="s">
         <v>182</v>
@@ -7291,16 +7718,17 @@
         <v>20</v>
       </c>
       <c r="G81">
-        <v>1.3455570189999999</v>
+        <f t="shared" si="1"/>
+        <v>1.5736980528638982</v>
       </c>
       <c r="H81">
-        <v>-1.01606</v>
+        <v>-2.9186292609175899</v>
       </c>
       <c r="I81">
-        <v>-0.75512000000000001</v>
+        <v>-1.8546310428522901</v>
       </c>
       <c r="J81">
-        <v>0.18079999999999999</v>
+        <v>0.19520000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -7308,7 +7736,7 @@
         <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C82" t="s">
         <v>183</v>
@@ -7323,16 +7751,17 @@
         <v>18</v>
       </c>
       <c r="G82">
-        <v>1.519902767</v>
+        <f t="shared" si="1"/>
+        <v>2.1349957691745223</v>
       </c>
       <c r="H82">
-        <v>-1.2463299999999999</v>
+        <v>-7.5883499830486398</v>
       </c>
       <c r="I82">
-        <v>-0.82001000000000002</v>
+        <v>-3.5542693304645798</v>
       </c>
       <c r="J82">
-        <v>2.3800000000000002E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -7340,7 +7769,7 @@
         <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C83" t="s">
         <v>182</v>
@@ -7355,16 +7784,17 @@
         <v>20</v>
       </c>
       <c r="G83">
-        <v>1.154339295</v>
+        <f t="shared" si="1"/>
+        <v>3.3312306401694398</v>
       </c>
       <c r="H83">
-        <v>-0.88014000000000003</v>
+        <v>-7.8258624373862604</v>
       </c>
       <c r="I83">
-        <v>-0.76246000000000003</v>
+        <v>-2.3492406508929702</v>
       </c>
       <c r="J83">
-        <v>0.38379999999999997</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -7372,7 +7802,7 @@
         <v>101</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
         <v>183</v>
@@ -7387,16 +7817,17 @@
         <v>19</v>
       </c>
       <c r="G84">
-        <v>0.33202407900000003</v>
+        <f t="shared" si="1"/>
+        <v>0.19954621645391221</v>
       </c>
       <c r="H84">
-        <v>-0.16861999999999999</v>
+        <v>-0.376366482528674</v>
       </c>
       <c r="I84">
-        <v>-0.50787000000000004</v>
+        <v>-1.88611184525065</v>
       </c>
       <c r="J84">
-        <v>0.75119999999999998</v>
+        <v>0.64639999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -7404,7 +7835,7 @@
         <v>101</v>
       </c>
       <c r="B85" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C85" t="s">
         <v>182</v>
@@ -7419,16 +7850,17 @@
         <v>20</v>
       </c>
       <c r="G85">
-        <v>1.0194488909999999</v>
+        <f t="shared" si="1"/>
+        <v>1.8204151527658843</v>
       </c>
       <c r="H85">
-        <v>-0.92095000000000005</v>
+        <v>-7.28044245747658</v>
       </c>
       <c r="I85">
-        <v>-0.90337999999999996</v>
+        <v>-3.99933083748226</v>
       </c>
       <c r="J85">
-        <v>0.49419999999999997</v>
+        <v>1.32E-2</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -7436,7 +7868,7 @@
         <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C86" t="s">
         <v>183</v>
@@ -7451,16 +7883,17 @@
         <v>19</v>
       </c>
       <c r="G86">
-        <v>1.223786885</v>
+        <f t="shared" si="1"/>
+        <v>1.319279658445653</v>
       </c>
       <c r="H86">
-        <v>-1.0243800000000001</v>
+        <v>-5.7394937329279401</v>
       </c>
       <c r="I86">
-        <v>-0.83706000000000003</v>
+        <v>-4.3504754251195603</v>
       </c>
       <c r="J86">
-        <v>0.186</v>
+        <v>0.2482</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -7483,16 +7916,17 @@
         <v>39</v>
       </c>
       <c r="G87">
-        <v>-5.2152842279999998</v>
+        <f t="shared" si="1"/>
+        <v>2.6741018182714638</v>
       </c>
       <c r="H87">
-        <v>9.1246670000000005</v>
+        <v>0.10142134597407999</v>
       </c>
       <c r="I87">
-        <v>-1.7496</v>
+        <v>3.7927256651595499E-2</v>
       </c>
       <c r="J87">
-        <v>0.92700000000000005</v>
+        <v>0.52400000000000002</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -7515,16 +7949,17 @@
         <v>41</v>
       </c>
       <c r="G88">
-        <v>0.75616177100000004</v>
+        <f t="shared" si="1"/>
+        <v>0.42691896907833227</v>
       </c>
       <c r="H88">
-        <v>-0.55674999999999997</v>
+        <v>-1.12883154894285</v>
       </c>
       <c r="I88">
-        <v>-0.73629</v>
+        <v>-2.6441353762749502</v>
       </c>
       <c r="J88">
-        <v>0.99239999999999995</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -7547,16 +7982,17 @@
         <v>32</v>
       </c>
       <c r="G89">
-        <v>1.0421373599999999</v>
+        <f t="shared" si="1"/>
+        <v>1.1017361451576724</v>
       </c>
       <c r="H89">
-        <v>-0.96616000000000002</v>
+        <v>-3.3626363924693501</v>
       </c>
       <c r="I89">
-        <v>-0.92710000000000004</v>
+        <v>-3.0521249640839501</v>
       </c>
       <c r="J89">
-        <v>0.40860000000000002</v>
+        <v>0.30399999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -7579,16 +8015,17 @@
         <v>32</v>
       </c>
       <c r="G90">
-        <v>1.111543181</v>
+        <f t="shared" si="1"/>
+        <v>1.349653923879319</v>
       </c>
       <c r="H90">
-        <v>-1.0245299999999999</v>
+        <v>-3.8946766961033599</v>
       </c>
       <c r="I90">
-        <v>-0.92171999999999998</v>
+        <v>-2.8856854540228101</v>
       </c>
       <c r="J90">
-        <v>0.21679999999999999</v>
+        <v>7.4800000000000005E-2</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -7611,20 +8048,1512 @@
         <v>27</v>
       </c>
       <c r="G91">
-        <v>1.0254693029999999</v>
+        <f t="shared" si="1"/>
+        <v>3.9931838002805677</v>
       </c>
       <c r="H91">
-        <v>-0.73233999999999999</v>
+        <v>-1.78515853812301</v>
       </c>
       <c r="I91">
-        <v>-0.71414999999999995</v>
+        <v>-0.447051432492935</v>
       </c>
       <c r="J91">
-        <v>0.48620000000000002</v>
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C91"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="170.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" t="s">
+        <v>217</v>
+      </c>
+      <c r="C78" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" t="s">
+        <v>90</v>
+      </c>
+      <c r="C81" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" t="s">
+        <v>91</v>
+      </c>
+      <c r="C82" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" t="s">
+        <v>94</v>
+      </c>
+      <c r="C85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" t="s">
+        <v>100</v>
+      </c>
+      <c r="C91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:A91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>